<commit_message>
weird comment in text removed
</commit_message>
<xml_diff>
--- a/data/Acculturation-Review-Codebook.xlsx
+++ b/data/Acculturation-Review-Codebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/PhD/Phd Research [shared]/What is integration/acculturation-review/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F9203A-1813-8D4A-9FFA-726A8D2D626F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD7F553-DE2D-0542-9B05-4270EC418503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20440" xr2:uid="{E23EBCE6-197B-BA40-9BB1-6A04FFA4E5A2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20440" activeTab="2" xr2:uid="{E23EBCE6-197B-BA40-9BB1-6A04FFA4E5A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Theoretical" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="216">
   <si>
     <t>Data/Code</t>
   </si>
@@ -855,7 +855,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="24">
     <dxf>
       <font>
         <b val="0"/>
@@ -873,7 +873,26 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1126,6 +1145,25 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1187,8 +1225,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="APA" pivot="0" count="2" xr9:uid="{25D85F84-CDCA-C84C-8F66-C484C7C29A08}">
-      <tableStyleElement type="wholeTable" dxfId="21"/>
-      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="wholeTable" dxfId="23"/>
+      <tableStyleElement type="headerRow" dxfId="22"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1203,40 +1241,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D289DD4F-79E8-3B49-9C6A-BA0AF7D8CAFA}" name="Table1" displayName="Table1" ref="A1:E21" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D289DD4F-79E8-3B49-9C6A-BA0AF7D8CAFA}" name="Table1" displayName="Table1" ref="A1:E21" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20">
   <autoFilter ref="A1:E21" xr:uid="{7BF059FB-9D8A-794A-90CE-2925C873644B}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{62FEADEA-D618-914E-A105-A854CBF7A05B}" name="Category" dataDxfId="0"/>
-    <tableColumn id="1" xr3:uid="{11448952-27C4-6F41-AC2D-C0585EAAFDA9}" name="Variable Name" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{EF68335B-4CF8-7447-83A2-688FEC56C83C}" name="Variable Type" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{247A667D-01D5-B242-8BE6-FE5E1C516DEA}" name="Data/Code" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00586C3B-88A9-9A45-A1E0-00D9084FDF9A}" name="Explanation/Comments" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{62FEADEA-D618-914E-A105-A854CBF7A05B}" name="Category" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{11448952-27C4-6F41-AC2D-C0585EAAFDA9}" name="Variable Name" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{EF68335B-4CF8-7447-83A2-688FEC56C83C}" name="Variable Type" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{247A667D-01D5-B242-8BE6-FE5E1C516DEA}" name="Data/Code" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00586C3B-88A9-9A45-A1E0-00D9084FDF9A}" name="Explanation/Comments" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="APA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{42C8167E-671F-5143-A129-FAE2C46148B4}" name="Table2" displayName="Table2" ref="A1:D35" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:D35" xr:uid="{3E9EE27E-2610-8645-BB18-981039699970}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{053E0949-7042-E34E-B84F-5BBD41E4B33D}" name="Variable Name" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{36C4CB90-F8B7-B848-B363-9E3F5EB30928}" name="Variable Type" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{FCCEC94A-2C8C-1043-B778-3B6DA2052506}" name="Data/Code" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{29C47257-F388-174B-8EFF-796863ED5B61}" name="Explanation/Comments" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{42C8167E-671F-5143-A129-FAE2C46148B4}" name="Table2" displayName="Table2" ref="A1:E35" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:E35" xr:uid="{3E9EE27E-2610-8645-BB18-981039699970}"/>
+  <tableColumns count="5">
+    <tableColumn id="5" xr3:uid="{9DD34F9A-8A84-D242-B1B2-189730F18BF7}" name="Category" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{053E0949-7042-E34E-B84F-5BBD41E4B33D}" name="Variable Name" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{36C4CB90-F8B7-B848-B363-9E3F5EB30928}" name="Variable Type" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{FCCEC94A-2C8C-1043-B778-3B6DA2052506}" name="Data/Code" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{29C47257-F388-174B-8EFF-796863ED5B61}" name="Explanation/Comments" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="APA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CC884A5F-193B-A04B-BBF8-C9422D049C5C}" name="Table3" displayName="Table3" ref="A1:D58" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:D58" xr:uid="{26D4140D-F977-3C42-BB41-DAD978358456}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3565A982-3668-3C48-BD40-67F9E1DDF2D2}" name="Variable Name" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{F38E3577-0643-7647-B908-AC7E06BB15B8}" name="Variable Type" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{3952ABFB-A00B-BA49-B312-8FF31B0BF787}" name="Data/Code" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{FA7D261A-5085-4049-9546-055293D0788E}" name="Explanation/Comments" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CC884A5F-193B-A04B-BBF8-C9422D049C5C}" name="Table3" displayName="Table3" ref="A1:E58" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:E58" xr:uid="{26D4140D-F977-3C42-BB41-DAD978358456}"/>
+  <tableColumns count="5">
+    <tableColumn id="5" xr3:uid="{EE931C16-A00A-6F4C-A7D7-36E4C8E0471F}" name="Category" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3565A982-3668-3C48-BD40-67F9E1DDF2D2}" name="Variable Name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{F38E3577-0643-7647-B908-AC7E06BB15B8}" name="Variable Type" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{3952ABFB-A00B-BA49-B312-8FF31B0BF787}" name="Data/Code" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{FA7D261A-5085-4049-9546-055293D0788E}" name="Explanation/Comments" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="APA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1541,13 +1581,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A1778F-82C8-E744-B43E-E361BE413F1C}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="21.5" style="3" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -1883,510 +1923,550 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA2A8D9-7D4A-1C40-9559-5776D5D4909D}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="9"/>
+    <col min="1" max="1" width="20.83203125" style="10" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>210</v>
-      </c>
       <c r="C2" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C3" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>210</v>
-      </c>
       <c r="C4" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>210</v>
-      </c>
       <c r="C5" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>210</v>
-      </c>
       <c r="C6" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>210</v>
-      </c>
       <c r="C7" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>210</v>
-      </c>
       <c r="C11" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>210</v>
-      </c>
       <c r="C12" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C13" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="E13" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C14" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C15" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C16" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C17" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="E17" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C18" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C19" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C20" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C21" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B22" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C22" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C23" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="E23" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B24" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C24" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="2:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B25" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C25" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="204" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="2:6" ht="306" x14ac:dyDescent="0.2">
+      <c r="B26" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="E26" s="10" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="119" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="2:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="B27" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C27" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="E27" s="10" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B28" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C28" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="2:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B29" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>210</v>
-      </c>
       <c r="C29" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="E29" s="10" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="2:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B30" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>210</v>
-      </c>
       <c r="C30" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="2:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="B31" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C31" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="E31" s="10" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="2:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="B32" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C32" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="2:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B33" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>210</v>
-      </c>
       <c r="C33" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="E33" s="10" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="2:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B34" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>210</v>
-      </c>
       <c r="C34" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="2:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B35" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="10" t="s">
-        <v>210</v>
-      </c>
       <c r="C35" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D35" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="E35" s="10" t="s">
         <v>187</v>
       </c>
+      <c r="F35" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2398,824 +2478,828 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0326CE-FBE4-7E4D-A111-DD058905A544}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="14"/>
+    <col min="1" max="1" width="17.83203125" style="14" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C2" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="B3" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C3" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="14" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="C4" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="14" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C5" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C6" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="B7" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C7" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="204" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:5" ht="306" x14ac:dyDescent="0.2">
+      <c r="B8" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>211</v>
-      </c>
       <c r="C8" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C9" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="B10" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C10" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="204" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:5" ht="306" x14ac:dyDescent="0.2">
+      <c r="B11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>211</v>
-      </c>
       <c r="C11" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C12" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C13" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="E13" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C14" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="C15" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="D15" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="C16" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="D16" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="E16" s="14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="C17" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="D17" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="E17" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="C18" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="D18" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="E18" s="14" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="C19" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="D19" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="E19" s="14" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="C20" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="D20" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="E20" s="14" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="14" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C21" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="E21" s="14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C22" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="E22" s="14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C23" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D23" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="E23" s="14" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C24" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D24" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="E24" s="14" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="14" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C25" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="E25" s="14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C26" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="E26" s="14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C27" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D27" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="E27" s="14" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
+    <row r="28" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B28" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C28" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="E28" s="14" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C29" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D29" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="E29" s="14" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C30" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D30" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="E30" s="14" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="14" t="s">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C31" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D31" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="E31" s="14" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A32" s="14" t="s">
+    <row r="32" spans="2:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="B32" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C32" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="E32" s="14" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="14" t="s">
+    <row r="33" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B33" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C33" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="E33" s="14" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A34" s="14" t="s">
+    <row r="34" spans="2:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="B34" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C34" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="E34" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C35" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D35" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="E35" s="14" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="14" t="s">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C36" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D36" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="E36" s="14" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="14" t="s">
+    <row r="37" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B37" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C37" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="E37" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="14" t="s">
+    <row r="38" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B38" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C38" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="E38" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="14" t="s">
+    <row r="39" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B39" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C39" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D39" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="E39" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="14" t="s">
+    <row r="40" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B40" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C40" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="E40" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A41" s="14" t="s">
+    <row r="41" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B41" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C41" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D41" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="E41" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A42" s="14" t="s">
+    <row r="42" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B42" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C42" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="E42" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A43" s="14" t="s">
+    <row r="43" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B43" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C43" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="E43" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A44" s="14" t="s">
+    <row r="44" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B44" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C44" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="E44" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A45" s="14" t="s">
+    <row r="45" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B45" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C45" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D45" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="E45" s="14" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="204" x14ac:dyDescent="0.2">
-      <c r="A46" s="14" t="s">
+    <row r="46" spans="2:5" ht="306" x14ac:dyDescent="0.2">
+      <c r="B46" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B46" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D46" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="E46" s="10" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="A47" s="14" t="s">
+    <row r="47" spans="2:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="B47" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B47" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C47" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D47" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="E47" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A48" s="14" t="s">
+    <row r="48" spans="2:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="B48" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C48" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D48" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="E48" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="14" t="s">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B49" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C49" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D49" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="D49" s="14" t="s">
+      <c r="E49" s="14" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="14" t="s">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B50" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B50" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C50" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D50" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="E50" s="14" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B51" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C51" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D51" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="E51" s="14" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="153" x14ac:dyDescent="0.2">
-      <c r="A52" s="14" t="s">
+    <row r="52" spans="2:5" ht="170" x14ac:dyDescent="0.2">
+      <c r="B52" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B52" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C52" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D52" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="E52" s="14" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="14" t="s">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B53" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B53" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C53" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D53" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="E53" s="14" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A54" s="14" t="s">
+    <row r="54" spans="2:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="B54" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C54" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D54" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="E54" s="14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A55" s="14" t="s">
+    <row r="55" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B55" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C55" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D55" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="E55" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="14" t="s">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B56" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C56" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D56" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="E56" s="14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="14" t="s">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B57" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B57" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C57" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D57" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="D57" s="14" t="s">
+      <c r="E57" s="14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="14" t="s">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B58" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="C58" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D58" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="E58" s="14" t="s">
         <v>137</v>
       </c>
     </row>

</xml_diff>